<commit_message>
Updated all files to support new uses
- Corrins get their autolevel skills added to their skillset
- Corrins get put into the correct gendered class if applicable
- Corrins do not get extra letters added onto their name if their name is less than 5 characters
</commit_message>
<xml_diff>
--- a/classes.xlsx
+++ b/classes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProjects\corrinquest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F691FAB0-AC33-431B-B62E-CD4D84A26969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C724D31-9C30-4D83-B2C9-7CA3989DEE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2325" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="428">
   <si>
     <t>Name</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Sword, Stone</t>
   </si>
   <si>
-    <t>['Nohr Noble' 'Hoshido Noble']</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>Sword</t>
   </si>
   <si>
-    <t>['Swordmaster' 'Master of Arms']</t>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
@@ -190,9 +184,6 @@
     <t>Lance</t>
   </si>
   <si>
-    <t>['Master of Arms' 'Merchant']</t>
-  </si>
-  <si>
     <t>6f</t>
   </si>
   <si>
@@ -211,9 +202,6 @@
     <t>Bow</t>
   </si>
   <si>
-    <t>['Merchant' 'Mechanist']</t>
-  </si>
-  <si>
     <t>4f</t>
   </si>
   <si>
@@ -232,9 +220,6 @@
     <t>Axe</t>
   </si>
   <si>
-    <t>['Oni Chieftain' 'Blacksmith']</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
@@ -286,9 +271,6 @@
     <t>40, 22, 15, 23, 22, 21, 22, 21</t>
   </si>
   <si>
-    <t>['Spear Master' 'Basara']</t>
-  </si>
-  <si>
     <t>2d</t>
   </si>
   <si>
@@ -337,9 +319,6 @@
     <t>Tome</t>
   </si>
   <si>
-    <t>['Onmyoji' 'Basara']</t>
-  </si>
-  <si>
     <t>31</t>
   </si>
   <si>
@@ -376,18 +355,12 @@
     <t>Staff</t>
   </si>
   <si>
-    <t>['Onmyoji' 'Great Master']</t>
-  </si>
-  <si>
     <t>35</t>
   </si>
   <si>
     <t>Shrine Maiden</t>
   </si>
   <si>
-    <t>['Onmyoji' 'Priestess']</t>
-  </si>
-  <si>
     <t>36</t>
   </si>
   <si>
@@ -439,9 +412,6 @@
     <t>35, 19, 16, 21, 23, 25, 18, 25</t>
   </si>
   <si>
-    <t>['Falcon Knight' 'Kinshi Knight']</t>
-  </si>
-  <si>
     <t>3b</t>
   </si>
   <si>
@@ -487,9 +457,6 @@
     <t>40, 21, 15, 23, 21, 20, 20, 17</t>
   </si>
   <si>
-    <t>['Sniper' 'Kinshi Knight']</t>
-  </si>
-  <si>
     <t>3f</t>
   </si>
   <si>
@@ -523,9 +490,6 @@
     <t>Hidden</t>
   </si>
   <si>
-    <t>['Master Ninja' 'Mechanist']</t>
-  </si>
-  <si>
     <t>4b</t>
   </si>
   <si>
@@ -580,9 +544,6 @@
     <t>Stone</t>
   </si>
   <si>
-    <t>['Nine-Tails']</t>
-  </si>
-  <si>
     <t>63</t>
   </si>
   <si>
@@ -613,9 +574,6 @@
     <t>Sword, Lance</t>
   </si>
   <si>
-    <t>['Paladin' 'Great Knight']</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -661,9 +619,6 @@
     <t>45, 24, 15, 22, 17, 22, 26, 18</t>
   </si>
   <si>
-    <t>['Great Knight' 'General']</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -697,9 +652,6 @@
     <t>45, 25, 15, 23, 22, 21, 19, 18</t>
   </si>
   <si>
-    <t>['Berserker' 'Hero']</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
@@ -730,9 +682,6 @@
     <t>40, 22, 15, 24, 22, 20, 21, 19</t>
   </si>
   <si>
-    <t>['Hero' 'Bow Knight']</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
@@ -781,9 +730,6 @@
     <t>35, 19, 18, 20, 24, 18, 17, 22</t>
   </si>
   <si>
-    <t>['Bow Knight' 'Adventurer']</t>
-  </si>
-  <si>
     <t>1b</t>
   </si>
   <si>
@@ -814,9 +760,6 @@
     <t>40, 22, 17, 21, 20, 19, 24, 15</t>
   </si>
   <si>
-    <t>['Wyvern Lord' 'Malig Knight']</t>
-  </si>
-  <si>
     <t>45</t>
   </si>
   <si>
@@ -862,9 +805,6 @@
     <t>35, 19, 24, 16, 19, 18, 19, 22</t>
   </si>
   <si>
-    <t>['Sorcerer' 'Dark Knight']</t>
-  </si>
-  <si>
     <t>55</t>
   </si>
   <si>
@@ -913,9 +853,6 @@
     <t>35, 16, 19, 24, 20, 23, 16, 21</t>
   </si>
   <si>
-    <t>['Maid' 'Butler' 'Strategist']</t>
-  </si>
-  <si>
     <t>5b</t>
   </si>
   <si>
@@ -970,9 +907,6 @@
     <t>45, 24, 15, 18, 22, 17, 21, 15</t>
   </si>
   <si>
-    <t>['Wolfssegner']</t>
-  </si>
-  <si>
     <t>5f</t>
   </si>
   <si>
@@ -1124,6 +1058,252 @@
   </si>
   <si>
     <t>7a</t>
+  </si>
+  <si>
+    <t>Nohr Noble, Hoshido Noble</t>
+  </si>
+  <si>
+    <t>Swordmaster, Master of Arms</t>
+  </si>
+  <si>
+    <t>Master of Arms, Merchant</t>
+  </si>
+  <si>
+    <t>Merchant, Mechanist</t>
+  </si>
+  <si>
+    <t>Oni Chieftain, Blacksmith</t>
+  </si>
+  <si>
+    <t>Spear Master, Basara</t>
+  </si>
+  <si>
+    <t>Onmyoji, Basara</t>
+  </si>
+  <si>
+    <t>Onmyoji, Great Master</t>
+  </si>
+  <si>
+    <t>Onmyoji, Priestess</t>
+  </si>
+  <si>
+    <t>Falcon Knight, Kinshi Knight</t>
+  </si>
+  <si>
+    <t>Sniper, Kinshi Knight</t>
+  </si>
+  <si>
+    <t>Master Ninja, Mechanist</t>
+  </si>
+  <si>
+    <t>Paladin, Great Knight</t>
+  </si>
+  <si>
+    <t>Great Knight, General</t>
+  </si>
+  <si>
+    <t>Hero, Bow Knight</t>
+  </si>
+  <si>
+    <t>Bow Knight, Adventurer</t>
+  </si>
+  <si>
+    <t>Wyvern Lord, Malig Knight</t>
+  </si>
+  <si>
+    <t>Sorcerer, Dark Knight</t>
+  </si>
+  <si>
+    <t>Maid, Butler, Strategist</t>
+  </si>
+  <si>
+    <t>Berserker, Hero</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Nobility, Dragon Fang</t>
+  </si>
+  <si>
+    <t>Dragon Ward, Hoshidan Unity</t>
+  </si>
+  <si>
+    <t>Draconic Hex, Nohrian Trust</t>
+  </si>
+  <si>
+    <t>Duelist's Blow, Vantage</t>
+  </si>
+  <si>
+    <t>Astra, Swordfaire</t>
+  </si>
+  <si>
+    <t>Seal Strength, Life and Death</t>
+  </si>
+  <si>
+    <t>Profiteer, Spendthrift</t>
+  </si>
+  <si>
+    <t>Aptitude, Underdog</t>
+  </si>
+  <si>
+    <t>Potent Potion, Quick Salve</t>
+  </si>
+  <si>
+    <t>Seal Resistance, Shove</t>
+  </si>
+  <si>
+    <t>Death Blow, Counter</t>
+  </si>
+  <si>
+    <t>Salvage Blow, Lancebreaker</t>
+  </si>
+  <si>
+    <t>Seal Defense, Swap</t>
+  </si>
+  <si>
+    <t>Seal Speed, Lancefaire</t>
+  </si>
+  <si>
+    <t>Rend Heaven, Quixotic</t>
+  </si>
+  <si>
+    <t>Magic +2, Future Sight</t>
+  </si>
+  <si>
+    <t>Rally Magic, Tomefaire</t>
+  </si>
+  <si>
+    <t>Miracle, Rally Luck</t>
+  </si>
+  <si>
+    <t>Renewal, Countermagic</t>
+  </si>
+  <si>
+    <t>Darting Blow, Camaraderie</t>
+  </si>
+  <si>
+    <t>Rally Speed, Warding Blow</t>
+  </si>
+  <si>
+    <t>Air Superiority, Amaterasu</t>
+  </si>
+  <si>
+    <t>Skill +2, Quick Draw</t>
+  </si>
+  <si>
+    <t>Certain Blow, Bowfaire</t>
+  </si>
+  <si>
+    <t>Locktouch, Poison Strike</t>
+  </si>
+  <si>
+    <t>Lethality, Shurikenfaire</t>
+  </si>
+  <si>
+    <t>Golembane, Replicate</t>
+  </si>
+  <si>
+    <t>Beastbane, Even Handed</t>
+  </si>
+  <si>
+    <t>Even Better, Grisly Wound</t>
+  </si>
+  <si>
+    <t>Elbow Room, Shelter</t>
+  </si>
+  <si>
+    <t>Defender, Aegis</t>
+  </si>
+  <si>
+    <t>Luna, Armored Blow</t>
+  </si>
+  <si>
+    <t>Defense +2, Natural Cover</t>
+  </si>
+  <si>
+    <t>Wary Fighter, Pavise</t>
+  </si>
+  <si>
+    <t>HP +5, Gamble</t>
+  </si>
+  <si>
+    <t>Rally Strength, Axefaire</t>
+  </si>
+  <si>
+    <t>Good Fortune, Strong Riposte</t>
+  </si>
+  <si>
+    <t>Sol, Axebreaker</t>
+  </si>
+  <si>
+    <t>Rally Skill, Shurikenbreaker</t>
+  </si>
+  <si>
+    <t>Locktouch, Movement +1</t>
+  </si>
+  <si>
+    <t>Lucky Seven, Pass</t>
+  </si>
+  <si>
+    <t>Strength +2, Lunge</t>
+  </si>
+  <si>
+    <t>Rally Defense, Swordbreaker</t>
+  </si>
+  <si>
+    <t>Savage Blow, Trample</t>
+  </si>
+  <si>
+    <t>Heartseeker, Malefic Aura</t>
+  </si>
+  <si>
+    <t>Vengeance, Bowbreaker</t>
+  </si>
+  <si>
+    <t>Seal Magic, Lifetaker</t>
+  </si>
+  <si>
+    <t>Resistance +2, Demoiselle</t>
+  </si>
+  <si>
+    <t>Rally Resistance, Inspiration</t>
+  </si>
+  <si>
+    <t>Live to Serve, Tomebreaker</t>
+  </si>
+  <si>
+    <t>Beastbane, Odd Shaped</t>
+  </si>
+  <si>
+    <t>Better Odds, Grisly Wound</t>
+  </si>
+  <si>
+    <t>Speed +2, Relief, Rally Movement, Galeforce</t>
+  </si>
+  <si>
+    <t>Even Keel, Iron Will, Clarity, Aggressor</t>
+  </si>
+  <si>
+    <t>Dual Striker, Charm, Aether, Awakening</t>
+  </si>
+  <si>
+    <t>Heavy Blade, Veteran Intuition, Aether, Strengthtaker</t>
+  </si>
+  <si>
+    <t>Tactical Advice, Solidarity, Ignis, Rally Spectrum</t>
+  </si>
+  <si>
+    <t>Shadowgift, Witch's Brew, Warp, Toxic Brew</t>
+  </si>
+  <si>
+    <t>Survey, Opportunity Shot, Rifled Barrel, Surefooted</t>
+  </si>
+  <si>
+    <t>Luck +4, Inspiring Song, Voice of Peace, Foreign Princess</t>
+  </si>
+  <si>
+    <t>Dancing Blade, Charm, Dual Guardsman, Speedtaker</t>
   </si>
 </sst>
 </file>
@@ -1486,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,9 +1681,10 @@
     <col min="5" max="5" width="24.85546875" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="29.85546875" customWidth="1"/>
+    <col min="9" max="9" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1528,8 +1709,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1549,1522 +1733,1714 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
+        <v>346</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>347</v>
+      </c>
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>34</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>37</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>39</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>42</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>43</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>45</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>47</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>48</v>
       </c>
-      <c r="F8" t="s">
+      <c r="I8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>49</v>
-      </c>
-      <c r="H8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>51</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
         <v>52</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>53</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
+        <v>348</v>
+      </c>
+      <c r="H9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>55</v>
-      </c>
-      <c r="G9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>58</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
         <v>59</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
+        <v>349</v>
+      </c>
+      <c r="H10" t="s">
         <v>60</v>
       </c>
-      <c r="E10" t="s">
+      <c r="I10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>61</v>
-      </c>
-      <c r="F10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>65</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" t="s">
+        <v>350</v>
+      </c>
+      <c r="H11" t="s">
         <v>66</v>
       </c>
-      <c r="D11" t="s">
+      <c r="I11" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>67</v>
-      </c>
-      <c r="E11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>72</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>73</v>
-      </c>
-      <c r="D12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>78</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>79</v>
-      </c>
-      <c r="D13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>84</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>351</v>
       </c>
       <c r="H14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="I14" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" t="s">
         <v>86</v>
       </c>
-      <c r="E15" t="s">
-        <v>92</v>
-      </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="I15" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="I16" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F17" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G17" t="s">
-        <v>105</v>
+        <v>352</v>
       </c>
       <c r="H17" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="I17" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="H18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="I18" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E19" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F19" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
+        <v>353</v>
       </c>
       <c r="H19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="I19" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" t="s">
+        <v>354</v>
+      </c>
+      <c r="H20" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>114</v>
-      </c>
-      <c r="D20" t="s">
-        <v>115</v>
-      </c>
-      <c r="E20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" t="s">
-        <v>117</v>
-      </c>
-      <c r="G20" t="s">
-        <v>121</v>
-      </c>
-      <c r="H20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>123</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E21" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F21" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="H21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="I21" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E22" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F22" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="H22" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="I22" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G23" t="s">
-        <v>139</v>
+        <v>355</v>
       </c>
       <c r="H23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="I23" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="E24" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F24" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="H24" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="I24" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D25" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E25" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="I25" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D26" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E26" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G26" t="s">
-        <v>155</v>
+        <v>356</v>
       </c>
       <c r="H26" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="I26" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="E27" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="F27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H27" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="I27" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D28" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E28" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F28" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="G28" t="s">
-        <v>167</v>
+        <v>357</v>
       </c>
       <c r="H28" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="I28" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D29" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E29" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F29" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="H29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="I29" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D30" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E30" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F30" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="H30" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="I30" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="D31" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E31" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="F31" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="G31" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H31" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="I31" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="D32" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E32" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="F32" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="H32" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="I32" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="D33" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="E33" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="F33" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="G33" t="s">
-        <v>197</v>
+        <v>358</v>
       </c>
       <c r="H33" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="I33" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="D34" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="E34" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="F34" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H34" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="I34" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="D35" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="E35" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="F35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H35" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+      <c r="I35" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="D36" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="E36" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G36" t="s">
-        <v>213</v>
+        <v>359</v>
       </c>
       <c r="H36" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="I36" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="D37" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="E37" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="F37" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="H37" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="I37" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="D38" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="E38" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="F38" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G38" t="s">
-        <v>225</v>
+        <v>365</v>
       </c>
       <c r="H38" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="I38" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="B39">
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="D39" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="E39" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="F39" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H39" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="I39" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="D40" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="E40" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="F40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>236</v>
+        <v>360</v>
       </c>
       <c r="H40" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="I40" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="D41" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="E41" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="F41" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H41" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="I41" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="D42" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="E42" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="F42" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="H42" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="I42" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="D43" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="E43" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="F43" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G43" t="s">
-        <v>253</v>
+        <v>361</v>
       </c>
       <c r="H43" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="I43" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="D44" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="E44" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="F44" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="H44" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="I44" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="D45" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="E45" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="F45" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G45" t="s">
-        <v>264</v>
+        <v>362</v>
       </c>
       <c r="H45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+      <c r="I45" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="D46" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="E46" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="F46" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="H46" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="I46" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="B47">
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="D47" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="E47" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="F47" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H47" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="I47" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="D48" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="E48" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="F48" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G48" t="s">
-        <v>280</v>
+        <v>363</v>
       </c>
       <c r="H48" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="I48" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="B49">
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="D49" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="E49" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="F49" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H49" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+      <c r="I49" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="D50" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="E50" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="F50" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="H50" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+      <c r="I50" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="D51" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="E51" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="F51" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G51" t="s">
-        <v>297</v>
+        <v>364</v>
       </c>
       <c r="H51" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+      <c r="I51" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="B52">
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="D52" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="E52" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="F52" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="H52" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="I52" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
       <c r="B53">
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="D53" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
       <c r="E53" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="F53" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="H53" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="I53" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="B54">
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="D54" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
       <c r="E54" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="F54" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="H54" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="I54" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="D55" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
       <c r="E55" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
       <c r="F55" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="G55" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="H55" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+      <c r="I55" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>318</v>
+        <v>296</v>
       </c>
       <c r="B56">
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
       <c r="D56" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
       <c r="E56" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="F56" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="H56" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="I56" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="B57">
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="D57" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
       <c r="E57" t="s">
-        <v>325</v>
+        <v>303</v>
       </c>
       <c r="F57" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H57" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="I57" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>327</v>
+        <v>305</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
       <c r="D58" t="s">
-        <v>329</v>
+        <v>307</v>
       </c>
       <c r="E58" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
       <c r="F58" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H58" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="I58" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>332</v>
+        <v>310</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>333</v>
+        <v>311</v>
       </c>
       <c r="D59" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
       <c r="E59" t="s">
-        <v>335</v>
+        <v>313</v>
       </c>
       <c r="F59" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="H59" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="I59" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B60">
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>339</v>
+        <v>317</v>
       </c>
       <c r="D60" t="s">
-        <v>340</v>
+        <v>318</v>
       </c>
       <c r="E60" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
       <c r="F60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H60" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="I60" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
       <c r="B61">
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
       <c r="D61" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
       <c r="E61" t="s">
-        <v>346</v>
+        <v>324</v>
       </c>
       <c r="F61" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H61" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+      <c r="I61" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="B62">
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
       <c r="D62" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="E62" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="F62" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H62" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+      <c r="I62" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>353</v>
+        <v>331</v>
       </c>
       <c r="B63">
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
       <c r="D63" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="E63" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="F63" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="H63" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="I63" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="B64">
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>359</v>
+        <v>337</v>
       </c>
       <c r="D64" t="s">
-        <v>360</v>
+        <v>338</v>
       </c>
       <c r="E64" t="s">
-        <v>361</v>
+        <v>339</v>
       </c>
       <c r="F64" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H64" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+      <c r="I64" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="B65">
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>364</v>
+        <v>342</v>
       </c>
       <c r="D65" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="E65" t="s">
-        <v>366</v>
+        <v>344</v>
       </c>
       <c r="F65" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H65" t="s">
-        <v>367</v>
+        <v>345</v>
+      </c>
+      <c r="I65" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set up weapon_distribution.xlsx and distribution.py for future automatic weapon distribution for Corrins
</commit_message>
<xml_diff>
--- a/classes.xlsx
+++ b/classes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProjects\corrinquest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProjects\Automatic-Corrin-Creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C724D31-9C30-4D83-B2C9-7CA3989DEE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3FEA45-DFDD-4B4A-8548-917B9369194C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2325" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="431">
   <si>
     <t>Name</t>
   </si>
@@ -1304,6 +1304,15 @@
   </si>
   <si>
     <t>Dancing Blade, Charm, Dual Guardsman, Speedtaker</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>Birthright</t>
+  </si>
+  <si>
+    <t>Conquest</t>
   </si>
 </sst>
 </file>
@@ -1666,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,7 +1693,7 @@
     <col min="9" max="9" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1712,8 +1721,11 @@
       <c r="I1" s="1" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1741,8 +1753,11 @@
       <c r="I2" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1767,8 +1782,11 @@
       <c r="I3" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1793,8 +1811,11 @@
       <c r="I4" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1822,8 +1843,11 @@
       <c r="I5" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1848,8 +1872,11 @@
       <c r="I6" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1874,8 +1901,11 @@
       <c r="I7" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1900,8 +1930,11 @@
       <c r="I8" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1929,8 +1962,11 @@
       <c r="I9" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -1958,8 +1994,11 @@
       <c r="I10" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1987,8 +2026,11 @@
       <c r="I11" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2013,8 +2055,11 @@
       <c r="I12" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -2039,8 +2084,11 @@
       <c r="I13" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -2068,8 +2116,11 @@
       <c r="I14" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -2094,8 +2145,11 @@
       <c r="I15" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -2120,8 +2174,11 @@
       <c r="I16" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
@@ -2149,8 +2206,11 @@
       <c r="I17" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -2175,8 +2235,11 @@
       <c r="I18" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>106</v>
       </c>
@@ -2204,8 +2267,11 @@
       <c r="I19" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -2233,8 +2299,11 @@
       <c r="I20" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -2259,8 +2328,11 @@
       <c r="I21" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -2285,8 +2357,11 @@
       <c r="I22" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -2314,8 +2389,11 @@
       <c r="I23" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -2340,8 +2418,11 @@
       <c r="I24" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>136</v>
       </c>
@@ -2366,8 +2447,11 @@
       <c r="I25" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>141</v>
       </c>
@@ -2395,8 +2479,11 @@
       <c r="I26" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>146</v>
       </c>
@@ -2421,8 +2508,11 @@
       <c r="I27" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>151</v>
       </c>
@@ -2450,8 +2540,11 @@
       <c r="I28" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>157</v>
       </c>
@@ -2476,8 +2569,11 @@
       <c r="I29" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>163</v>
       </c>
@@ -2502,8 +2598,11 @@
       <c r="I30" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>169</v>
       </c>
@@ -2531,8 +2630,11 @@
       <c r="I31" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>175</v>
       </c>
@@ -2557,8 +2659,11 @@
       <c r="I32" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>179</v>
       </c>
@@ -2586,8 +2691,11 @@
       <c r="I33" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>185</v>
       </c>
@@ -2612,8 +2720,11 @@
       <c r="I34" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -2638,8 +2749,11 @@
       <c r="I35" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>195</v>
       </c>
@@ -2667,8 +2781,11 @@
       <c r="I36" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>200</v>
       </c>
@@ -2693,8 +2810,11 @@
       <c r="I37" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>206</v>
       </c>
@@ -2722,8 +2842,11 @@
       <c r="I38" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>211</v>
       </c>
@@ -2748,8 +2871,11 @@
       <c r="I39" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>216</v>
       </c>
@@ -2777,8 +2903,11 @@
       <c r="I40" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>221</v>
       </c>
@@ -2803,8 +2932,11 @@
       <c r="I41" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>226</v>
       </c>
@@ -2829,8 +2961,11 @@
       <c r="I42" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>232</v>
       </c>
@@ -2858,8 +2993,11 @@
       <c r="I43" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>237</v>
       </c>
@@ -2884,8 +3022,11 @@
       <c r="I44" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>242</v>
       </c>
@@ -2913,8 +3054,11 @@
       <c r="I45" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>247</v>
       </c>
@@ -2939,8 +3083,11 @@
       <c r="I46" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>252</v>
       </c>
@@ -2965,8 +3112,11 @@
       <c r="I47" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>257</v>
       </c>
@@ -2994,8 +3144,11 @@
       <c r="I48" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>262</v>
       </c>
@@ -3020,8 +3173,11 @@
       <c r="I49" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>267</v>
       </c>
@@ -3046,8 +3202,11 @@
       <c r="I50" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>273</v>
       </c>
@@ -3075,8 +3234,11 @@
       <c r="I51" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>278</v>
       </c>
@@ -3101,8 +3263,11 @@
       <c r="I52" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>283</v>
       </c>
@@ -3127,8 +3292,11 @@
       <c r="I53" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>289</v>
       </c>
@@ -3153,8 +3321,11 @@
       <c r="I54" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>291</v>
       </c>
@@ -3182,8 +3353,11 @@
       <c r="I55" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>296</v>
       </c>
@@ -3208,8 +3382,11 @@
       <c r="I56" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>300</v>
       </c>
@@ -3234,8 +3411,11 @@
       <c r="I57" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>305</v>
       </c>
@@ -3260,8 +3440,11 @@
       <c r="I58" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>310</v>
       </c>
@@ -3286,8 +3469,11 @@
       <c r="I59" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>316</v>
       </c>
@@ -3312,8 +3498,11 @@
       <c r="I60" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>321</v>
       </c>
@@ -3338,8 +3527,11 @@
       <c r="I61" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>326</v>
       </c>
@@ -3364,8 +3556,11 @@
       <c r="I62" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>331</v>
       </c>
@@ -3390,8 +3585,11 @@
       <c r="I63" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>336</v>
       </c>
@@ -3416,8 +3614,11 @@
       <c r="I64" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>341</v>
       </c>
@@ -3441,6 +3642,9 @@
       </c>
       <c r="I65" t="s">
         <v>425</v>
+      </c>
+      <c r="J65" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added gain_formulas.xlsx and weapon_ranks.py, files that are used to automatically give Corrins autolevelled weapon ranks appropriate for their join times.
</commit_message>
<xml_diff>
--- a/classes.xlsx
+++ b/classes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProjects\Automatic-Corrin-Creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3FEA45-DFDD-4B4A-8548-917B9369194C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432A413B-EC38-4BA1-BAD0-B854E8F7EACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2325" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="436">
   <si>
     <t>Name</t>
   </si>
@@ -1313,6 +1313,21 @@
   </si>
   <si>
     <t>Conquest</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -1368,9 +1383,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1675,10 +1693,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,11 +1708,13 @@
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" customWidth="1"/>
-    <col min="9" max="9" width="49.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" customWidth="1"/>
+    <col min="10" max="17" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1721,11 +1742,35 @@
       <c r="I1" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1754,10 +1799,34 @@
         <v>367</v>
       </c>
       <c r="J2" t="s">
+        <v>432</v>
+      </c>
+      <c r="K2" t="s">
+        <v>431</v>
+      </c>
+      <c r="L2" t="s">
+        <v>431</v>
+      </c>
+      <c r="M2" t="s">
+        <v>431</v>
+      </c>
+      <c r="N2" t="s">
+        <v>431</v>
+      </c>
+      <c r="O2" t="s">
+        <v>431</v>
+      </c>
+      <c r="P2" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>432</v>
+      </c>
+      <c r="R2" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1783,10 +1852,34 @@
         <v>368</v>
       </c>
       <c r="J3" t="s">
+        <v>433</v>
+      </c>
+      <c r="K3" t="s">
+        <v>431</v>
+      </c>
+      <c r="L3" t="s">
+        <v>431</v>
+      </c>
+      <c r="M3" t="s">
+        <v>431</v>
+      </c>
+      <c r="N3" t="s">
+        <v>431</v>
+      </c>
+      <c r="O3" t="s">
+        <v>431</v>
+      </c>
+      <c r="P3" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>433</v>
+      </c>
+      <c r="R3" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1812,10 +1905,34 @@
         <v>369</v>
       </c>
       <c r="J4" t="s">
+        <v>433</v>
+      </c>
+      <c r="K4" t="s">
+        <v>431</v>
+      </c>
+      <c r="L4" t="s">
+        <v>431</v>
+      </c>
+      <c r="M4" t="s">
+        <v>431</v>
+      </c>
+      <c r="N4" t="s">
+        <v>432</v>
+      </c>
+      <c r="O4" t="s">
+        <v>431</v>
+      </c>
+      <c r="P4" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>433</v>
+      </c>
+      <c r="R4" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1844,10 +1961,34 @@
         <v>370</v>
       </c>
       <c r="J5" t="s">
+        <v>432</v>
+      </c>
+      <c r="K5" t="s">
+        <v>431</v>
+      </c>
+      <c r="L5" t="s">
+        <v>431</v>
+      </c>
+      <c r="M5" t="s">
+        <v>431</v>
+      </c>
+      <c r="N5" t="s">
+        <v>431</v>
+      </c>
+      <c r="O5" t="s">
+        <v>431</v>
+      </c>
+      <c r="P5" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>431</v>
+      </c>
+      <c r="R5" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1873,10 +2014,34 @@
         <v>371</v>
       </c>
       <c r="J6" t="s">
+        <v>434</v>
+      </c>
+      <c r="K6" t="s">
+        <v>431</v>
+      </c>
+      <c r="L6" t="s">
+        <v>431</v>
+      </c>
+      <c r="M6" t="s">
+        <v>431</v>
+      </c>
+      <c r="N6" t="s">
+        <v>431</v>
+      </c>
+      <c r="O6" t="s">
+        <v>431</v>
+      </c>
+      <c r="P6" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>431</v>
+      </c>
+      <c r="R6" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1902,10 +2067,34 @@
         <v>372</v>
       </c>
       <c r="J7" t="s">
+        <v>433</v>
+      </c>
+      <c r="K7" t="s">
+        <v>432</v>
+      </c>
+      <c r="L7" t="s">
+        <v>432</v>
+      </c>
+      <c r="M7" t="s">
+        <v>431</v>
+      </c>
+      <c r="N7" t="s">
+        <v>431</v>
+      </c>
+      <c r="O7" t="s">
+        <v>431</v>
+      </c>
+      <c r="P7" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>431</v>
+      </c>
+      <c r="R7" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1931,10 +2120,34 @@
         <v>373</v>
       </c>
       <c r="J8" t="s">
+        <v>431</v>
+      </c>
+      <c r="K8" t="s">
+        <v>432</v>
+      </c>
+      <c r="L8" t="s">
+        <v>431</v>
+      </c>
+      <c r="M8" t="s">
+        <v>433</v>
+      </c>
+      <c r="N8" t="s">
+        <v>431</v>
+      </c>
+      <c r="O8" t="s">
+        <v>431</v>
+      </c>
+      <c r="P8" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>431</v>
+      </c>
+      <c r="R8" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1963,10 +2176,34 @@
         <v>374</v>
       </c>
       <c r="J9" t="s">
+        <v>431</v>
+      </c>
+      <c r="K9" t="s">
+        <v>435</v>
+      </c>
+      <c r="L9" t="s">
+        <v>431</v>
+      </c>
+      <c r="M9" t="s">
+        <v>431</v>
+      </c>
+      <c r="N9" t="s">
+        <v>431</v>
+      </c>
+      <c r="O9" t="s">
+        <v>431</v>
+      </c>
+      <c r="P9" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>431</v>
+      </c>
+      <c r="R9" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -1995,10 +2232,34 @@
         <v>375</v>
       </c>
       <c r="J10" t="s">
+        <v>431</v>
+      </c>
+      <c r="K10" t="s">
+        <v>431</v>
+      </c>
+      <c r="L10" t="s">
+        <v>431</v>
+      </c>
+      <c r="M10" t="s">
+        <v>432</v>
+      </c>
+      <c r="N10" t="s">
+        <v>431</v>
+      </c>
+      <c r="O10" t="s">
+        <v>431</v>
+      </c>
+      <c r="P10" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>431</v>
+      </c>
+      <c r="R10" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -2027,10 +2288,34 @@
         <v>376</v>
       </c>
       <c r="J11" t="s">
+        <v>431</v>
+      </c>
+      <c r="K11" t="s">
+        <v>431</v>
+      </c>
+      <c r="L11" t="s">
+        <v>432</v>
+      </c>
+      <c r="M11" t="s">
+        <v>431</v>
+      </c>
+      <c r="N11" t="s">
+        <v>431</v>
+      </c>
+      <c r="O11" t="s">
+        <v>431</v>
+      </c>
+      <c r="P11" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>431</v>
+      </c>
+      <c r="R11" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2056,10 +2341,34 @@
         <v>377</v>
       </c>
       <c r="J12" t="s">
+        <v>431</v>
+      </c>
+      <c r="K12" t="s">
+        <v>431</v>
+      </c>
+      <c r="L12" t="s">
+        <v>433</v>
+      </c>
+      <c r="M12" t="s">
+        <v>431</v>
+      </c>
+      <c r="N12" t="s">
+        <v>432</v>
+      </c>
+      <c r="O12" t="s">
+        <v>431</v>
+      </c>
+      <c r="P12" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>431</v>
+      </c>
+      <c r="R12" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -2085,10 +2394,34 @@
         <v>378</v>
       </c>
       <c r="J13" t="s">
+        <v>432</v>
+      </c>
+      <c r="K13" t="s">
+        <v>431</v>
+      </c>
+      <c r="L13" t="s">
+        <v>433</v>
+      </c>
+      <c r="M13" t="s">
+        <v>431</v>
+      </c>
+      <c r="N13" t="s">
+        <v>431</v>
+      </c>
+      <c r="O13" t="s">
+        <v>431</v>
+      </c>
+      <c r="P13" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>431</v>
+      </c>
+      <c r="R13" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -2117,10 +2450,34 @@
         <v>379</v>
       </c>
       <c r="J14" t="s">
+        <v>431</v>
+      </c>
+      <c r="K14" t="s">
+        <v>432</v>
+      </c>
+      <c r="L14" t="s">
+        <v>431</v>
+      </c>
+      <c r="M14" t="s">
+        <v>431</v>
+      </c>
+      <c r="N14" t="s">
+        <v>431</v>
+      </c>
+      <c r="O14" t="s">
+        <v>431</v>
+      </c>
+      <c r="P14" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>431</v>
+      </c>
+      <c r="R14" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -2146,10 +2503,34 @@
         <v>380</v>
       </c>
       <c r="J15" t="s">
+        <v>431</v>
+      </c>
+      <c r="K15" t="s">
+        <v>434</v>
+      </c>
+      <c r="L15" t="s">
+        <v>431</v>
+      </c>
+      <c r="M15" t="s">
+        <v>431</v>
+      </c>
+      <c r="N15" t="s">
+        <v>431</v>
+      </c>
+      <c r="O15" t="s">
+        <v>431</v>
+      </c>
+      <c r="P15" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>431</v>
+      </c>
+      <c r="R15" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -2175,10 +2556,34 @@
         <v>381</v>
       </c>
       <c r="J16" t="s">
+        <v>431</v>
+      </c>
+      <c r="K16" t="s">
+        <v>433</v>
+      </c>
+      <c r="L16" t="s">
+        <v>431</v>
+      </c>
+      <c r="M16" t="s">
+        <v>431</v>
+      </c>
+      <c r="N16" t="s">
+        <v>432</v>
+      </c>
+      <c r="O16" t="s">
+        <v>431</v>
+      </c>
+      <c r="P16" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>431</v>
+      </c>
+      <c r="R16" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
@@ -2207,10 +2612,34 @@
         <v>382</v>
       </c>
       <c r="J17" t="s">
+        <v>431</v>
+      </c>
+      <c r="K17" t="s">
+        <v>431</v>
+      </c>
+      <c r="L17" t="s">
+        <v>431</v>
+      </c>
+      <c r="M17" t="s">
+        <v>431</v>
+      </c>
+      <c r="N17" t="s">
+        <v>432</v>
+      </c>
+      <c r="O17" t="s">
+        <v>431</v>
+      </c>
+      <c r="P17" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>431</v>
+      </c>
+      <c r="R17" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -2236,10 +2665,34 @@
         <v>383</v>
       </c>
       <c r="J18" t="s">
+        <v>431</v>
+      </c>
+      <c r="K18" t="s">
+        <v>431</v>
+      </c>
+      <c r="L18" t="s">
+        <v>431</v>
+      </c>
+      <c r="M18" t="s">
+        <v>431</v>
+      </c>
+      <c r="N18" t="s">
+        <v>433</v>
+      </c>
+      <c r="O18" t="s">
+        <v>431</v>
+      </c>
+      <c r="P18" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>431</v>
+      </c>
+      <c r="R18" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>106</v>
       </c>
@@ -2268,10 +2721,34 @@
         <v>384</v>
       </c>
       <c r="J19" t="s">
+        <v>431</v>
+      </c>
+      <c r="K19" t="s">
+        <v>431</v>
+      </c>
+      <c r="L19" t="s">
+        <v>431</v>
+      </c>
+      <c r="M19" t="s">
+        <v>431</v>
+      </c>
+      <c r="N19" t="s">
+        <v>431</v>
+      </c>
+      <c r="O19" t="s">
+        <v>431</v>
+      </c>
+      <c r="P19" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>431</v>
+      </c>
+      <c r="R19" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -2300,10 +2777,34 @@
         <v>384</v>
       </c>
       <c r="J20" t="s">
+        <v>431</v>
+      </c>
+      <c r="K20" t="s">
+        <v>431</v>
+      </c>
+      <c r="L20" t="s">
+        <v>431</v>
+      </c>
+      <c r="M20" t="s">
+        <v>431</v>
+      </c>
+      <c r="N20" t="s">
+        <v>431</v>
+      </c>
+      <c r="O20" t="s">
+        <v>431</v>
+      </c>
+      <c r="P20" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>431</v>
+      </c>
+      <c r="R20" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -2329,10 +2830,34 @@
         <v>385</v>
       </c>
       <c r="J21" t="s">
+        <v>431</v>
+      </c>
+      <c r="K21" t="s">
+        <v>432</v>
+      </c>
+      <c r="L21" t="s">
+        <v>431</v>
+      </c>
+      <c r="M21" t="s">
+        <v>431</v>
+      </c>
+      <c r="N21" t="s">
+        <v>431</v>
+      </c>
+      <c r="O21" t="s">
+        <v>431</v>
+      </c>
+      <c r="P21" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>431</v>
+      </c>
+      <c r="R21" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -2358,10 +2883,34 @@
         <v>385</v>
       </c>
       <c r="J22" t="s">
+        <v>431</v>
+      </c>
+      <c r="K22" t="s">
+        <v>431</v>
+      </c>
+      <c r="L22" t="s">
+        <v>431</v>
+      </c>
+      <c r="M22" t="s">
+        <v>432</v>
+      </c>
+      <c r="N22" t="s">
+        <v>431</v>
+      </c>
+      <c r="O22" t="s">
+        <v>431</v>
+      </c>
+      <c r="P22" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>431</v>
+      </c>
+      <c r="R22" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -2390,10 +2939,34 @@
         <v>386</v>
       </c>
       <c r="J23" t="s">
+        <v>431</v>
+      </c>
+      <c r="K23" t="s">
+        <v>432</v>
+      </c>
+      <c r="L23" t="s">
+        <v>431</v>
+      </c>
+      <c r="M23" t="s">
+        <v>431</v>
+      </c>
+      <c r="N23" t="s">
+        <v>431</v>
+      </c>
+      <c r="O23" t="s">
+        <v>431</v>
+      </c>
+      <c r="P23" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>431</v>
+      </c>
+      <c r="R23" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -2419,10 +2992,34 @@
         <v>387</v>
       </c>
       <c r="J24" t="s">
+        <v>431</v>
+      </c>
+      <c r="K24" t="s">
+        <v>433</v>
+      </c>
+      <c r="L24" t="s">
+        <v>431</v>
+      </c>
+      <c r="M24" t="s">
+        <v>431</v>
+      </c>
+      <c r="N24" t="s">
+        <v>431</v>
+      </c>
+      <c r="O24" t="s">
+        <v>431</v>
+      </c>
+      <c r="P24" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>431</v>
+      </c>
+      <c r="R24" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>136</v>
       </c>
@@ -2448,10 +3045,34 @@
         <v>388</v>
       </c>
       <c r="J25" t="s">
+        <v>431</v>
+      </c>
+      <c r="K25" t="s">
+        <v>432</v>
+      </c>
+      <c r="L25" t="s">
+        <v>431</v>
+      </c>
+      <c r="M25" t="s">
+        <v>433</v>
+      </c>
+      <c r="N25" t="s">
+        <v>431</v>
+      </c>
+      <c r="O25" t="s">
+        <v>431</v>
+      </c>
+      <c r="P25" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>431</v>
+      </c>
+      <c r="R25" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>141</v>
       </c>
@@ -2480,10 +3101,34 @@
         <v>389</v>
       </c>
       <c r="J26" t="s">
+        <v>431</v>
+      </c>
+      <c r="K26" t="s">
+        <v>431</v>
+      </c>
+      <c r="L26" t="s">
+        <v>431</v>
+      </c>
+      <c r="M26" t="s">
+        <v>432</v>
+      </c>
+      <c r="N26" t="s">
+        <v>431</v>
+      </c>
+      <c r="O26" t="s">
+        <v>431</v>
+      </c>
+      <c r="P26" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>431</v>
+      </c>
+      <c r="R26" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>146</v>
       </c>
@@ -2509,10 +3154,34 @@
         <v>390</v>
       </c>
       <c r="J27" t="s">
+        <v>431</v>
+      </c>
+      <c r="K27" t="s">
+        <v>431</v>
+      </c>
+      <c r="L27" t="s">
+        <v>431</v>
+      </c>
+      <c r="M27" t="s">
+        <v>434</v>
+      </c>
+      <c r="N27" t="s">
+        <v>431</v>
+      </c>
+      <c r="O27" t="s">
+        <v>431</v>
+      </c>
+      <c r="P27" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>431</v>
+      </c>
+      <c r="R27" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>151</v>
       </c>
@@ -2541,10 +3210,34 @@
         <v>391</v>
       </c>
       <c r="J28" t="s">
+        <v>431</v>
+      </c>
+      <c r="K28" t="s">
+        <v>431</v>
+      </c>
+      <c r="L28" t="s">
+        <v>431</v>
+      </c>
+      <c r="M28" t="s">
+        <v>431</v>
+      </c>
+      <c r="N28" t="s">
+        <v>431</v>
+      </c>
+      <c r="O28" t="s">
+        <v>432</v>
+      </c>
+      <c r="P28" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>431</v>
+      </c>
+      <c r="R28" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>157</v>
       </c>
@@ -2570,10 +3263,34 @@
         <v>392</v>
       </c>
       <c r="J29" t="s">
+        <v>432</v>
+      </c>
+      <c r="K29" t="s">
+        <v>431</v>
+      </c>
+      <c r="L29" t="s">
+        <v>431</v>
+      </c>
+      <c r="M29" t="s">
+        <v>431</v>
+      </c>
+      <c r="N29" t="s">
+        <v>431</v>
+      </c>
+      <c r="O29" t="s">
+        <v>434</v>
+      </c>
+      <c r="P29" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>431</v>
+      </c>
+      <c r="R29" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>163</v>
       </c>
@@ -2599,10 +3316,34 @@
         <v>393</v>
       </c>
       <c r="J30" t="s">
+        <v>431</v>
+      </c>
+      <c r="K30" t="s">
+        <v>431</v>
+      </c>
+      <c r="L30" t="s">
+        <v>431</v>
+      </c>
+      <c r="M30" t="s">
+        <v>432</v>
+      </c>
+      <c r="N30" t="s">
+        <v>431</v>
+      </c>
+      <c r="O30" t="s">
+        <v>433</v>
+      </c>
+      <c r="P30" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>431</v>
+      </c>
+      <c r="R30" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>169</v>
       </c>
@@ -2631,10 +3372,34 @@
         <v>394</v>
       </c>
       <c r="J31" t="s">
+        <v>431</v>
+      </c>
+      <c r="K31" t="s">
+        <v>431</v>
+      </c>
+      <c r="L31" t="s">
+        <v>431</v>
+      </c>
+      <c r="M31" t="s">
+        <v>431</v>
+      </c>
+      <c r="N31" t="s">
+        <v>431</v>
+      </c>
+      <c r="O31" t="s">
+        <v>431</v>
+      </c>
+      <c r="P31" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>432</v>
+      </c>
+      <c r="R31" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>175</v>
       </c>
@@ -2660,10 +3425,34 @@
         <v>395</v>
       </c>
       <c r="J32" t="s">
+        <v>431</v>
+      </c>
+      <c r="K32" t="s">
+        <v>431</v>
+      </c>
+      <c r="L32" t="s">
+        <v>431</v>
+      </c>
+      <c r="M32" t="s">
+        <v>431</v>
+      </c>
+      <c r="N32" t="s">
+        <v>431</v>
+      </c>
+      <c r="O32" t="s">
+        <v>431</v>
+      </c>
+      <c r="P32" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>434</v>
+      </c>
+      <c r="R32" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>179</v>
       </c>
@@ -2692,10 +3481,34 @@
         <v>396</v>
       </c>
       <c r="J33" t="s">
+        <v>432</v>
+      </c>
+      <c r="K33" t="s">
+        <v>432</v>
+      </c>
+      <c r="L33" t="s">
+        <v>431</v>
+      </c>
+      <c r="M33" t="s">
+        <v>431</v>
+      </c>
+      <c r="N33" t="s">
+        <v>431</v>
+      </c>
+      <c r="O33" t="s">
+        <v>431</v>
+      </c>
+      <c r="P33" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>431</v>
+      </c>
+      <c r="R33" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>185</v>
       </c>
@@ -2721,10 +3534,34 @@
         <v>397</v>
       </c>
       <c r="J34" t="s">
+        <v>433</v>
+      </c>
+      <c r="K34" t="s">
+        <v>433</v>
+      </c>
+      <c r="L34" t="s">
+        <v>431</v>
+      </c>
+      <c r="M34" t="s">
+        <v>431</v>
+      </c>
+      <c r="N34" t="s">
+        <v>431</v>
+      </c>
+      <c r="O34" t="s">
+        <v>431</v>
+      </c>
+      <c r="P34" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>431</v>
+      </c>
+      <c r="R34" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -2750,10 +3587,34 @@
         <v>398</v>
       </c>
       <c r="J35" t="s">
+        <v>432</v>
+      </c>
+      <c r="K35" t="s">
+        <v>433</v>
+      </c>
+      <c r="L35" t="s">
+        <v>432</v>
+      </c>
+      <c r="M35" t="s">
+        <v>431</v>
+      </c>
+      <c r="N35" t="s">
+        <v>431</v>
+      </c>
+      <c r="O35" t="s">
+        <v>431</v>
+      </c>
+      <c r="P35" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>431</v>
+      </c>
+      <c r="R35" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>195</v>
       </c>
@@ -2782,10 +3643,34 @@
         <v>399</v>
       </c>
       <c r="J36" t="s">
+        <v>431</v>
+      </c>
+      <c r="K36" t="s">
+        <v>432</v>
+      </c>
+      <c r="L36" t="s">
+        <v>431</v>
+      </c>
+      <c r="M36" t="s">
+        <v>431</v>
+      </c>
+      <c r="N36" t="s">
+        <v>431</v>
+      </c>
+      <c r="O36" t="s">
+        <v>431</v>
+      </c>
+      <c r="P36" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>431</v>
+      </c>
+      <c r="R36" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>200</v>
       </c>
@@ -2811,10 +3696,34 @@
         <v>400</v>
       </c>
       <c r="J37" t="s">
+        <v>431</v>
+      </c>
+      <c r="K37" t="s">
+        <v>433</v>
+      </c>
+      <c r="L37" t="s">
+        <v>432</v>
+      </c>
+      <c r="M37" t="s">
+        <v>431</v>
+      </c>
+      <c r="N37" t="s">
+        <v>431</v>
+      </c>
+      <c r="O37" t="s">
+        <v>431</v>
+      </c>
+      <c r="P37" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>431</v>
+      </c>
+      <c r="R37" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>206</v>
       </c>
@@ -2843,10 +3752,34 @@
         <v>401</v>
       </c>
       <c r="J38" t="s">
+        <v>431</v>
+      </c>
+      <c r="K38" t="s">
+        <v>431</v>
+      </c>
+      <c r="L38" t="s">
+        <v>432</v>
+      </c>
+      <c r="M38" t="s">
+        <v>431</v>
+      </c>
+      <c r="N38" t="s">
+        <v>431</v>
+      </c>
+      <c r="O38" t="s">
+        <v>431</v>
+      </c>
+      <c r="P38" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>431</v>
+      </c>
+      <c r="R38" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>211</v>
       </c>
@@ -2872,10 +3805,34 @@
         <v>402</v>
       </c>
       <c r="J39" t="s">
+        <v>431</v>
+      </c>
+      <c r="K39" t="s">
+        <v>431</v>
+      </c>
+      <c r="L39" t="s">
+        <v>434</v>
+      </c>
+      <c r="M39" t="s">
+        <v>431</v>
+      </c>
+      <c r="N39" t="s">
+        <v>431</v>
+      </c>
+      <c r="O39" t="s">
+        <v>431</v>
+      </c>
+      <c r="P39" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>431</v>
+      </c>
+      <c r="R39" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>216</v>
       </c>
@@ -2904,10 +3861,34 @@
         <v>403</v>
       </c>
       <c r="J40" t="s">
+        <v>432</v>
+      </c>
+      <c r="K40" t="s">
+        <v>431</v>
+      </c>
+      <c r="L40" t="s">
+        <v>431</v>
+      </c>
+      <c r="M40" t="s">
+        <v>431</v>
+      </c>
+      <c r="N40" t="s">
+        <v>431</v>
+      </c>
+      <c r="O40" t="s">
+        <v>431</v>
+      </c>
+      <c r="P40" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>431</v>
+      </c>
+      <c r="R40" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>221</v>
       </c>
@@ -2933,10 +3914,34 @@
         <v>404</v>
       </c>
       <c r="J41" t="s">
+        <v>433</v>
+      </c>
+      <c r="K41" t="s">
+        <v>431</v>
+      </c>
+      <c r="L41" t="s">
+        <v>432</v>
+      </c>
+      <c r="M41" t="s">
+        <v>431</v>
+      </c>
+      <c r="N41" t="s">
+        <v>431</v>
+      </c>
+      <c r="O41" t="s">
+        <v>431</v>
+      </c>
+      <c r="P41" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>431</v>
+      </c>
+      <c r="R41" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>226</v>
       </c>
@@ -2962,10 +3967,34 @@
         <v>405</v>
       </c>
       <c r="J42" t="s">
+        <v>432</v>
+      </c>
+      <c r="K42" t="s">
+        <v>431</v>
+      </c>
+      <c r="L42" t="s">
+        <v>431</v>
+      </c>
+      <c r="M42" t="s">
+        <v>433</v>
+      </c>
+      <c r="N42" t="s">
+        <v>431</v>
+      </c>
+      <c r="O42" t="s">
+        <v>431</v>
+      </c>
+      <c r="P42" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>431</v>
+      </c>
+      <c r="R42" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>232</v>
       </c>
@@ -2994,10 +4023,34 @@
         <v>406</v>
       </c>
       <c r="J43" t="s">
+        <v>431</v>
+      </c>
+      <c r="K43" t="s">
+        <v>431</v>
+      </c>
+      <c r="L43" t="s">
+        <v>431</v>
+      </c>
+      <c r="M43" t="s">
+        <v>432</v>
+      </c>
+      <c r="N43" t="s">
+        <v>431</v>
+      </c>
+      <c r="O43" t="s">
+        <v>431</v>
+      </c>
+      <c r="P43" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>431</v>
+      </c>
+      <c r="R43" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>237</v>
       </c>
@@ -3023,10 +4076,34 @@
         <v>407</v>
       </c>
       <c r="J44" t="s">
+        <v>431</v>
+      </c>
+      <c r="K44" t="s">
+        <v>431</v>
+      </c>
+      <c r="L44" t="s">
+        <v>431</v>
+      </c>
+      <c r="M44" t="s">
+        <v>433</v>
+      </c>
+      <c r="N44" t="s">
+        <v>431</v>
+      </c>
+      <c r="O44" t="s">
+        <v>431</v>
+      </c>
+      <c r="P44" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>431</v>
+      </c>
+      <c r="R44" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>242</v>
       </c>
@@ -3055,10 +4132,34 @@
         <v>408</v>
       </c>
       <c r="J45" t="s">
+        <v>431</v>
+      </c>
+      <c r="K45" t="s">
+        <v>431</v>
+      </c>
+      <c r="L45" t="s">
+        <v>432</v>
+      </c>
+      <c r="M45" t="s">
+        <v>431</v>
+      </c>
+      <c r="N45" t="s">
+        <v>431</v>
+      </c>
+      <c r="O45" t="s">
+        <v>431</v>
+      </c>
+      <c r="P45" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>431</v>
+      </c>
+      <c r="R45" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>247</v>
       </c>
@@ -3084,10 +4185,34 @@
         <v>409</v>
       </c>
       <c r="J46" t="s">
+        <v>431</v>
+      </c>
+      <c r="K46" t="s">
+        <v>432</v>
+      </c>
+      <c r="L46" t="s">
+        <v>433</v>
+      </c>
+      <c r="M46" t="s">
+        <v>431</v>
+      </c>
+      <c r="N46" t="s">
+        <v>431</v>
+      </c>
+      <c r="O46" t="s">
+        <v>431</v>
+      </c>
+      <c r="P46" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>431</v>
+      </c>
+      <c r="R46" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>252</v>
       </c>
@@ -3113,10 +4238,34 @@
         <v>410</v>
       </c>
       <c r="J47" t="s">
+        <v>431</v>
+      </c>
+      <c r="K47" t="s">
+        <v>431</v>
+      </c>
+      <c r="L47" t="s">
+        <v>433</v>
+      </c>
+      <c r="M47" t="s">
+        <v>431</v>
+      </c>
+      <c r="N47" t="s">
+        <v>432</v>
+      </c>
+      <c r="O47" t="s">
+        <v>431</v>
+      </c>
+      <c r="P47" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>431</v>
+      </c>
+      <c r="R47" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>257</v>
       </c>
@@ -3145,10 +4294,34 @@
         <v>411</v>
       </c>
       <c r="J48" t="s">
+        <v>431</v>
+      </c>
+      <c r="K48" t="s">
+        <v>431</v>
+      </c>
+      <c r="L48" t="s">
+        <v>431</v>
+      </c>
+      <c r="M48" t="s">
+        <v>431</v>
+      </c>
+      <c r="N48" t="s">
+        <v>432</v>
+      </c>
+      <c r="O48" t="s">
+        <v>431</v>
+      </c>
+      <c r="P48" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>431</v>
+      </c>
+      <c r="R48" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>262</v>
       </c>
@@ -3174,10 +4347,34 @@
         <v>412</v>
       </c>
       <c r="J49" t="s">
+        <v>431</v>
+      </c>
+      <c r="K49" t="s">
+        <v>431</v>
+      </c>
+      <c r="L49" t="s">
+        <v>431</v>
+      </c>
+      <c r="M49" t="s">
+        <v>431</v>
+      </c>
+      <c r="N49" t="s">
+        <v>434</v>
+      </c>
+      <c r="O49" t="s">
+        <v>431</v>
+      </c>
+      <c r="P49" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>431</v>
+      </c>
+      <c r="R49" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>267</v>
       </c>
@@ -3203,10 +4400,34 @@
         <v>413</v>
       </c>
       <c r="J50" t="s">
+        <v>432</v>
+      </c>
+      <c r="K50" t="s">
+        <v>431</v>
+      </c>
+      <c r="L50" t="s">
+        <v>431</v>
+      </c>
+      <c r="M50" t="s">
+        <v>431</v>
+      </c>
+      <c r="N50" t="s">
+        <v>433</v>
+      </c>
+      <c r="O50" t="s">
+        <v>431</v>
+      </c>
+      <c r="P50" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>431</v>
+      </c>
+      <c r="R50" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>273</v>
       </c>
@@ -3235,10 +4456,34 @@
         <v>414</v>
       </c>
       <c r="J51" t="s">
+        <v>431</v>
+      </c>
+      <c r="K51" t="s">
+        <v>431</v>
+      </c>
+      <c r="L51" t="s">
+        <v>431</v>
+      </c>
+      <c r="M51" t="s">
+        <v>431</v>
+      </c>
+      <c r="N51" t="s">
+        <v>431</v>
+      </c>
+      <c r="O51" t="s">
+        <v>431</v>
+      </c>
+      <c r="P51" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>431</v>
+      </c>
+      <c r="R51" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>278</v>
       </c>
@@ -3264,10 +4509,34 @@
         <v>415</v>
       </c>
       <c r="J52" t="s">
+        <v>431</v>
+      </c>
+      <c r="K52" t="s">
+        <v>431</v>
+      </c>
+      <c r="L52" t="s">
+        <v>431</v>
+      </c>
+      <c r="M52" t="s">
+        <v>431</v>
+      </c>
+      <c r="N52" t="s">
+        <v>432</v>
+      </c>
+      <c r="O52" t="s">
+        <v>431</v>
+      </c>
+      <c r="P52" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>431</v>
+      </c>
+      <c r="R52" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>283</v>
       </c>
@@ -3293,10 +4562,34 @@
         <v>416</v>
       </c>
       <c r="J53" t="s">
+        <v>431</v>
+      </c>
+      <c r="K53" t="s">
+        <v>431</v>
+      </c>
+      <c r="L53" t="s">
+        <v>431</v>
+      </c>
+      <c r="M53" t="s">
+        <v>431</v>
+      </c>
+      <c r="N53" t="s">
+        <v>431</v>
+      </c>
+      <c r="O53" t="s">
+        <v>432</v>
+      </c>
+      <c r="P53" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>431</v>
+      </c>
+      <c r="R53" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>289</v>
       </c>
@@ -3322,10 +4615,34 @@
         <v>416</v>
       </c>
       <c r="J54" t="s">
+        <v>431</v>
+      </c>
+      <c r="K54" t="s">
+        <v>431</v>
+      </c>
+      <c r="L54" t="s">
+        <v>431</v>
+      </c>
+      <c r="M54" t="s">
+        <v>431</v>
+      </c>
+      <c r="N54" t="s">
+        <v>431</v>
+      </c>
+      <c r="O54" t="s">
+        <v>432</v>
+      </c>
+      <c r="P54" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>431</v>
+      </c>
+      <c r="R54" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>291</v>
       </c>
@@ -3354,10 +4671,34 @@
         <v>417</v>
       </c>
       <c r="J55" t="s">
+        <v>431</v>
+      </c>
+      <c r="K55" t="s">
+        <v>431</v>
+      </c>
+      <c r="L55" t="s">
+        <v>431</v>
+      </c>
+      <c r="M55" t="s">
+        <v>431</v>
+      </c>
+      <c r="N55" t="s">
+        <v>431</v>
+      </c>
+      <c r="O55" t="s">
+        <v>431</v>
+      </c>
+      <c r="P55" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>432</v>
+      </c>
+      <c r="R55" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>296</v>
       </c>
@@ -3383,10 +4724,34 @@
         <v>418</v>
       </c>
       <c r="J56" t="s">
+        <v>431</v>
+      </c>
+      <c r="K56" t="s">
+        <v>431</v>
+      </c>
+      <c r="L56" t="s">
+        <v>431</v>
+      </c>
+      <c r="M56" t="s">
+        <v>431</v>
+      </c>
+      <c r="N56" t="s">
+        <v>431</v>
+      </c>
+      <c r="O56" t="s">
+        <v>431</v>
+      </c>
+      <c r="P56" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>434</v>
+      </c>
+      <c r="R56" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>300</v>
       </c>
@@ -3412,10 +4777,34 @@
         <v>426</v>
       </c>
       <c r="J57" t="s">
+        <v>431</v>
+      </c>
+      <c r="K57" t="s">
+        <v>435</v>
+      </c>
+      <c r="L57" t="s">
+        <v>431</v>
+      </c>
+      <c r="M57" t="s">
+        <v>431</v>
+      </c>
+      <c r="N57" t="s">
+        <v>431</v>
+      </c>
+      <c r="O57" t="s">
+        <v>431</v>
+      </c>
+      <c r="P57" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>431</v>
+      </c>
+      <c r="R57" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>305</v>
       </c>
@@ -3441,10 +4830,34 @@
         <v>419</v>
       </c>
       <c r="J58" t="s">
+        <v>431</v>
+      </c>
+      <c r="K58" t="s">
+        <v>432</v>
+      </c>
+      <c r="L58" t="s">
+        <v>431</v>
+      </c>
+      <c r="M58" t="s">
+        <v>431</v>
+      </c>
+      <c r="N58" t="s">
+        <v>433</v>
+      </c>
+      <c r="O58" t="s">
+        <v>431</v>
+      </c>
+      <c r="P58" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>431</v>
+      </c>
+      <c r="R58" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>310</v>
       </c>
@@ -3470,10 +4883,34 @@
         <v>420</v>
       </c>
       <c r="J59" t="s">
+        <v>433</v>
+      </c>
+      <c r="K59" t="s">
+        <v>431</v>
+      </c>
+      <c r="L59" t="s">
+        <v>432</v>
+      </c>
+      <c r="M59" t="s">
+        <v>431</v>
+      </c>
+      <c r="N59" t="s">
+        <v>431</v>
+      </c>
+      <c r="O59" t="s">
+        <v>432</v>
+      </c>
+      <c r="P59" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>431</v>
+      </c>
+      <c r="R59" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>316</v>
       </c>
@@ -3499,10 +4936,34 @@
         <v>427</v>
       </c>
       <c r="J60" t="s">
+        <v>434</v>
+      </c>
+      <c r="K60" t="s">
+        <v>431</v>
+      </c>
+      <c r="L60" t="s">
+        <v>431</v>
+      </c>
+      <c r="M60" t="s">
+        <v>431</v>
+      </c>
+      <c r="N60" t="s">
+        <v>431</v>
+      </c>
+      <c r="O60" t="s">
+        <v>431</v>
+      </c>
+      <c r="P60" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>431</v>
+      </c>
+      <c r="R60" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>321</v>
       </c>
@@ -3528,10 +4989,34 @@
         <v>421</v>
       </c>
       <c r="J61" t="s">
+        <v>433</v>
+      </c>
+      <c r="K61" t="s">
+        <v>432</v>
+      </c>
+      <c r="L61" t="s">
+        <v>431</v>
+      </c>
+      <c r="M61" t="s">
+        <v>431</v>
+      </c>
+      <c r="N61" t="s">
+        <v>431</v>
+      </c>
+      <c r="O61" t="s">
+        <v>431</v>
+      </c>
+      <c r="P61" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>431</v>
+      </c>
+      <c r="R61" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>326</v>
       </c>
@@ -3557,10 +5042,34 @@
         <v>422</v>
       </c>
       <c r="J62" t="s">
+        <v>433</v>
+      </c>
+      <c r="K62" t="s">
+        <v>431</v>
+      </c>
+      <c r="L62" t="s">
+        <v>432</v>
+      </c>
+      <c r="M62" t="s">
+        <v>431</v>
+      </c>
+      <c r="N62" t="s">
+        <v>431</v>
+      </c>
+      <c r="O62" t="s">
+        <v>431</v>
+      </c>
+      <c r="P62" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>431</v>
+      </c>
+      <c r="R62" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>331</v>
       </c>
@@ -3586,10 +5095,34 @@
         <v>423</v>
       </c>
       <c r="J63" t="s">
+        <v>432</v>
+      </c>
+      <c r="K63" t="s">
+        <v>431</v>
+      </c>
+      <c r="L63" t="s">
+        <v>431</v>
+      </c>
+      <c r="M63" t="s">
+        <v>431</v>
+      </c>
+      <c r="N63" t="s">
+        <v>433</v>
+      </c>
+      <c r="O63" t="s">
+        <v>431</v>
+      </c>
+      <c r="P63" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>431</v>
+      </c>
+      <c r="R63" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>336</v>
       </c>
@@ -3615,10 +5148,34 @@
         <v>424</v>
       </c>
       <c r="J64" t="s">
+        <v>431</v>
+      </c>
+      <c r="K64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L64" t="s">
+        <v>431</v>
+      </c>
+      <c r="M64" t="s">
+        <v>431</v>
+      </c>
+      <c r="N64" t="s">
+        <v>434</v>
+      </c>
+      <c r="O64" t="s">
+        <v>431</v>
+      </c>
+      <c r="P64" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>431</v>
+      </c>
+      <c r="R64" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>341</v>
       </c>
@@ -3644,6 +5201,30 @@
         <v>425</v>
       </c>
       <c r="J65" t="s">
+        <v>431</v>
+      </c>
+      <c r="K65" t="s">
+        <v>431</v>
+      </c>
+      <c r="L65" t="s">
+        <v>431</v>
+      </c>
+      <c r="M65" t="s">
+        <v>432</v>
+      </c>
+      <c r="N65" t="s">
+        <v>431</v>
+      </c>
+      <c r="O65" t="s">
+        <v>431</v>
+      </c>
+      <c r="P65" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>431</v>
+      </c>
+      <c r="R65" t="s">
         <v>430</v>
       </c>
     </row>

</xml_diff>